<commit_message>
classify topic of question then selected columns
</commit_message>
<xml_diff>
--- a/Experiments/EXP_LLM_SQLresult.xlsx
+++ b/Experiments/EXP_LLM_SQLresult.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', 447), ('2022-08', 259)]</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(178992.0,)]</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', 30075.0), ('2022-08', 30045.0)]</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(13.825421897546896,)]</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[(13.825421897546896,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', 47.61290322580645), ('2022-08', 55.1578947368421)]</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[(10.0, '2022-07-01'), (10.0, '2022-07-02'), (4.0, '2022-07-03'), (9.0, '2022-07-04'), (12.0, '2022-07-05'), (21.0, '2022-07-06'), (28.0, '2022-07-07'), (89.0, '2022-07-08'), (50.0, '2022-07-09'), (21.0, '2022-07-10'), (39.0, '2022-07-11'), (41.0, '2022-07-12'), (24.0, '2022-07-13'), (28.0, '2022-07-14'), (260.0, '2022-07-15'), (171.0, '2022-07-16'), (62.0, '2022-07-17'), (80.0, '2022-07-18'), (53.0, '2022-07-19'), (59.0, '2022-07-20'), (53.0, '2022-07-21'), (44.0, '2022-07-22'), (40.0, '2022-07-23'), (16.0, '2022-07-24'), (46.0, '2022-07-25'), (52.0, '2022-07-26'), (34.0, '2022-07-27'), (33.0, '2022-07-28'), (22.0, '2022-07-29'), (25.0, '2022-07-30'), (40.0, '2022-07-31'), (32.0, '2022-08-01'), (28.0, '2022-08-02'), (38.0, '2022-08-03'), (46.0, '2022-08-04'), (37.0, '2022-08-05'), (21.0, '2022-08-06'), (14.0, '2022-08-07'), (25.0, '2022-08-08'), (30.0, '2022-08-09'), (32.0, '2022-08-10'), (27.0, '2022-08-11'), (14.0, '2022-08-12'), (14.0, '2022-08-13'), (13.0, '2022-08-14'), (27.0, '2022-08-15'), (35.0, '2022-08-16'), (45.0, '2022-08-17'), (7.0, '2022-08-18'), (563.0, '2022-08-19')]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(437,)]</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(221,)]</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[(3,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(1.305,)]</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(39,)]</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1378,7 +1378,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(None,)]</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-07', None), ('2022-08', None), ('2022-08', None), ('2022-08', None), ('2022-07', None), ('2022-08', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-07', None), ('2022-08', None), ('2022-08', None), ('2022-08', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-08', None), ('2022-08', None), ('2022-07', None), ('2022-08', None), ('2022-08', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-07', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-07', None), ('2022-07', None), ('2022-08', None), ('2022-08', None)]</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[(None, 50)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', None), ('2022-08', None)]</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07-01', 195), ('2022-07-02', 195), ('2022-07-03', 195), ('2022-07-04', 196), ('2022-07-05', 196), ('2022-07-06', 196), ('2022-07-07', 198), ('2022-07-08', 223), ('2022-07-09', 249), ('2022-07-10', 254), ('2022-07-11', 266), ('2022-07-12', 275), ('2022-07-13', 278), ('2022-07-14', 285), ('2022-07-15', 471), ('2022-07-16', 595), ('2022-07-17', 621), ('2022-07-18', 646), ('2022-07-19', 658), ('2022-07-20', 672), ('2022-07-21', 680), ('2022-07-22', 686), ('2022-07-23', 691), ('2022-07-24', 693), ('2022-07-25', 701), ('2022-07-26', 710), ('2022-07-27', 712), ('2022-07-28', 712), ('2022-07-29', 714), ('2022-07-30', 716), ('2022-07-31', 725), ('2022-08-01', 728), ('2022-08-02', 731), ('2022-08-03', 735), ('2022-08-04', 741), ('2022-08-05', 753), ('2022-08-06', 755), ('2022-08-07', 756), ('2022-08-08', 758), ('2022-08-09', 763), ('2022-08-10', 766), ('2022-08-11', 768), ('2022-08-12', 768), ('2022-08-13', 768), ('2022-08-14', 769), ('2022-08-15', 770), ('2022-08-16', 778), ('2022-08-17', 783), ('2022-08-18', 792), ('2022-08-19', 1247)]</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>[(50,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', 2.4516129032258065), ('2022-08', 3.4473684210526314)]</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-07', 7), ('2022-08', 10)]</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(3,)]</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>[(50,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>[(50,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>[(13.825421897546896,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>[(5,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>[(50,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -3043,7 +3043,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(6,), (37,), (12,), (9,), (17,), (5,), (10,), (5,), (5,), (3,), (18,), (8,), (9,), (7,), (5,), (8,), (10,), (7,), (11,)]</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>[(50,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3579,7 +3579,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3665,7 +3665,7 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>[('2022-08-14',), ('2022-07-27',), ('2022-07-16',), ('2022-08-18',), ('2022-07-26',)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>[('2022-07-06',), ('2022-07-01',), ('2022-07-08',)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-05-23', 1), ('2022-05-24', 6), ('2022-05-25', 4), ('2022-05-26', 2), ('2022-05-27', 7), ('2022-05-28', 1), ('2022-05-30', 2)]</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -4012,7 +4012,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('2022-05', 22)]</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('0198f28f3b2d07688c66a6aabf1a6c18', '2022-05-25T20:57:03.975+0000'), ('0412E26637DD42D6B3DCE818E153495B', '2022-05-24T17:22:44.809+0000'), ('2618A002B7F649AD88D1E3E2AE0C9D34', '2022-05-30T15:05:31.311+0000'), ('474ae23630781fc3b8d08ee6bc8038a4', '2022-05-28T16:07:04.821+0000'), ('5AF61BAC90A94DF2A25B432D527FD88E', '2022-05-30T17:02:09.937+0000'), ('5C7F578875D448F9B17AB7512FEF401B', '2022-05-25T01:32:49.712+0000'), ('70b17c4bfcebf709bc1a45f98b5d1a39', '2022-05-27T14:52:14.617+0000'), ('76487BD129734D0BA622A19E3348EDFB', '2022-05-27T13:15:59.241+0000'), ('78995275425D44D5B4418B639FE41B3A', '2022-05-24T18:45:55.027+0000'), ('78e36f49bff175a8fe7bd910af2016d9', '2022-05-27T15:19:40.929+0000'), ('850BC09AF0CE488AB8DC4C70B39DC35F', '2022-05-24T12:06:51.837+0000'), ('8984e7e0d2373e31fdece9a43e47e99e', '2022-05-23T17:46:44.976+0000'), ('89970B97EFAA447F85C61A10C70ED0B0', '2022-05-26T16:26:17.768+0000'), ('9CD78C6F93AC42B7804C376277750F4A', '2022-05-24T16:20:38.551+0000'), ('9DE0535A75E7420DAFC90F1C5B67E2D7', '2022-05-24T01:45:43.556+0000'), ('A387790874A44EF9A9F5D6B5E1885656', '2022-05-25T15:27:58.272+0000'), ('D0662C11CE7E454ABCD9732FCBC6CD92', '2022-05-25T22:19:40.994+0000'), ('D23C83AC69D74FAC836FB942CECE6DFA', '2022-05-27T15:21:19.018+0000'), ('D7D907A202874EA4A4A3F48E2BF6186F', '2022-05-24T14:51:38.809+0000'), ('EC05EE85432F44BE81415BDB06E0714B', '2022-05-27T14:46:27.893+0000'), ('F51A60AC085F4416B246F636099DAB85', '2022-05-27T18:34:10.527+0000'), ('daf44a8e8f02d47895ef65027e06428c', '2022-05-27T10:26:03.568+0000')]</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4376,7 +4376,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(22,)]</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -4386,7 +4386,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>[(223,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>[(1000,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4852,7 +4852,7 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>[('2022-05', 1000)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4942,7 +4942,7 @@
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>[(25,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -5115,7 +5115,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('0198f28f3b2d07688c66a6aabf1a6c18', 2), ('0412E26637DD42D6B3DCE818E153495B', 1), ('2618A002B7F649AD88D1E3E2AE0C9D34', 1), ('474ae23630781fc3b8d08ee6bc8038a4', 1), ('5AF61BAC90A94DF2A25B432D527FD88E', 3), ('5C7F578875D448F9B17AB7512FEF401B', 2), ('70b17c4bfcebf709bc1a45f98b5d1a39', 2), ('76487BD129734D0BA622A19E3348EDFB', 1), ('78995275425D44D5B4418B639FE41B3A', 1), ('78e36f49bff175a8fe7bd910af2016d9', 1), ('850BC09AF0CE488AB8DC4C70B39DC35F', 1), ('8984e7e0d2373e31fdece9a43e47e99e', 2), ('89970B97EFAA447F85C61A10C70ED0B0', 3), ('9CD78C6F93AC42B7804C376277750F4A', 1), ('9DE0535A75E7420DAFC90F1C5B67E2D7', 2), ('A387790874A44EF9A9F5D6B5E1885656', 4), ('D0662C11CE7E454ABCD9732FCBC6CD92', 1), ('D23C83AC69D74FAC836FB942CECE6DFA', 2), ('D7D907A202874EA4A4A3F48E2BF6186F', 1), ('EC05EE85432F44BE81415BDB06E0714B', 2), ('F51A60AC085F4416B246F636099DAB85', 1), ('d75e40462e09492af8788e72df9aa0e4', 1), ('daf44a8e8f02d47895ef65027e06428c', 1), ('fb0d14acd0679ee580e8fa800d8476b7', 1)]</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -5125,7 +5125,7 @@
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -5215,7 +5215,7 @@
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>[(25,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -5860,7 +5860,7 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>[(31, '2022-05-23'), (122, '2022-05-24'), (157, '2022-05-25'), (144, '2022-05-26'), (383, '2022-05-27'), (19, '2022-05-28'), (5, '2022-05-29'), (139, '2022-05-30')]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -6049,7 +6049,7 @@
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>[('2022-05-27',)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -6130,7 +6130,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(1.2432432432432432,)]</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>[(3618.109,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -6218,7 +6218,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(1.4285714285714286,)]</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -6228,7 +6228,7 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>[(inf,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>[(inf,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -6401,7 +6401,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(0.5714285714285714,)]</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -6411,7 +6411,7 @@
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>[(3618.109,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -6502,7 +6502,7 @@
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -6683,7 +6683,7 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -6771,7 +6771,7 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>[(25,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -6849,7 +6849,7 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('pointx_dealoftheday_landing', 277, 0), ('screen_view', 194, 0), ('user_engagement', 177, 0), ('mypointx_landing', 47, 0), ('session_start', 38, 0), ('pointx_home_bottom_bar', 25, 0), ('payatmcht_landing', 23, 0), ('pointx_view_mypoint', 19, 0), ('pointx_payandmerchant_bottom_bar', 15, 0), ('pointx_mypointx_bottom_bar', 14, 0)]</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
@@ -6859,7 +6859,7 @@
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -6955,7 +6955,7 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -7045,7 +7045,7 @@
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -7135,7 +7135,7 @@
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -7227,7 +7227,7 @@
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -7317,7 +7317,7 @@
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -7409,7 +7409,7 @@
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -7499,7 +7499,7 @@
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -7589,7 +7589,7 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>[(861,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>[(861,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -7953,7 +7953,7 @@
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -8045,7 +8045,7 @@
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -8229,7 +8229,7 @@
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -8319,7 +8319,7 @@
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -8409,7 +8409,7 @@
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>[(25,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
@@ -8501,7 +8501,7 @@
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -8594,7 +8594,7 @@
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
@@ -8675,7 +8675,7 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(307.6,)]</t>
         </is>
       </c>
       <c r="N92" t="inlineStr">
@@ -8685,7 +8685,7 @@
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P92" t="inlineStr">
@@ -8766,7 +8766,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('1', 0), ('Pixel 6', 0), ('Redmi Note 5', 0), ('SH-01L', 0), ('SM-A526B', 0), ('SM-F711B', 0), ('SM-G985F', 0), ('SM-G998B', 0), ('SM-S908E', 0), ('iPhone', 0), ('iPhone 11', 0), ('iPhone 11 Pro Max', 0), ('iPhone 12 Pro', 0), ('iPhone 13 Pro', 0), ('iPhone 13 Pro Max', 0), ('iPhone 8 Plus', 0), ('iPhone XR', 0), ('iPhone XS', 0)]</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -8776,7 +8776,7 @@
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>[('mobile', 1000)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P93" t="inlineStr">
@@ -8867,7 +8867,7 @@
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P94" t="inlineStr">
@@ -9064,7 +9064,7 @@
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P96" t="inlineStr">
@@ -9155,7 +9155,7 @@
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P97" t="inlineStr">
@@ -9246,7 +9246,7 @@
       </c>
       <c r="O98" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P98" t="inlineStr">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('Bangkok', 19), ('Chon Buri', 1), ('Nonthaburi', 2), ('Phra Nakhon Si Ayutthaya', 1)]</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
@@ -9348,7 +9348,7 @@
       </c>
       <c r="O99" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P99" t="inlineStr">
@@ -9440,7 +9440,7 @@
       </c>
       <c r="O100" t="inlineStr">
         <is>
-          <t>[(None,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P100" t="inlineStr">
@@ -9536,7 +9536,7 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P101" t="inlineStr">
@@ -9628,7 +9628,7 @@
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>[(3618.109,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P102" t="inlineStr">
@@ -9719,7 +9719,7 @@
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P103" t="inlineStr">
@@ -9811,7 +9811,7 @@
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>[(0,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P104" t="inlineStr">
@@ -9890,7 +9890,7 @@
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[(25,)]</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
@@ -9900,7 +9900,7 @@
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>[(1,)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P105" t="inlineStr">
@@ -9978,7 +9978,7 @@
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>CANNOT FETCHING DATA</t>
+          <t>[('session_start',), ('screen_view',), ('user_engagement',), ('pointx_dealoftheday_landing',), ('mypointx_landing',), ('pointx_home_bottom_bar',), ('pointx_view_mypoint',), ('payatmcht_landing',), ('virtualmall_landing',), ('pointx_virtualmall_bottom_bar',)]</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -9988,7 +9988,7 @@
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>[('pointx_payandmerchant_bottom_bar',), ('mypointx_landing',), ('pointx_home_bottom_bar',), ('screen_view',), ('mypointx_landing',), ('user_engagement',), ('mypointx_landing',), ('screen_view',), ('virtualmall_landing',), ('user_engagement',)]</t>
+          <t>CANNOT FETCHING DATA</t>
         </is>
       </c>
       <c r="P106" t="inlineStr">

</xml_diff>